<commit_message>
Add comprehensive statistical analysis report generation script and output file
</commit_message>
<xml_diff>
--- a/flow.xlsx
+++ b/flow.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11018"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11026"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michalfischbein/projects/FINAL PROJECT/trial files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michalfischbein/projects/final project flow/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C690A7B-A751-E040-AD51-C69F0CF9D258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23DF4E57-1DF8-A942-B679-DE1D6B4D9826}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="340" yWindow="500" windowWidth="28100" windowHeight="16100" xr2:uid="{0BA294BD-C3A5-D442-BD2F-C06C5A9B2827}"/>
   </bookViews>
@@ -498,7 +498,7 @@
   <dimension ref="F2:M20"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
added yaml, updated py's
</commit_message>
<xml_diff>
--- a/flow.xlsx
+++ b/flow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michalfischbein/projects/final project flow/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23DF4E57-1DF8-A942-B679-DE1D6B4D9826}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59517651-C60A-0242-B071-6CD6D641D52F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="340" yWindow="500" windowWidth="28100" windowHeight="16100" xr2:uid="{0BA294BD-C3A5-D442-BD2F-C06C5A9B2827}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
   <si>
     <t>שלב</t>
   </si>
@@ -120,6 +120,12 @@
   </si>
   <si>
     <t>גישה לאינטרנט לחפש רעיונות</t>
+  </si>
+  <si>
+    <t>צוות 1</t>
+  </si>
+  <si>
+    <t>צוות 2</t>
   </si>
 </sst>
 </file>
@@ -497,8 +503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{497A6988-A12C-F541-BFDF-410B958FC78E}">
   <dimension ref="F2:M20"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="L6" sqref="F6:L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -545,7 +551,7 @@
     </row>
     <row r="6" spans="6:13" ht="37" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F6" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="G6" t="s">
         <v>8</v>
@@ -583,7 +589,7 @@
     </row>
     <row r="11" spans="6:13" ht="17" x14ac:dyDescent="0.2">
       <c r="F11" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="G11" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
updated yaml, corrected code,
</commit_message>
<xml_diff>
--- a/flow.xlsx
+++ b/flow.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11102"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michalfischbein/projects/final project flow/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10E5B1D3-5169-DD42-9FA3-DE21A46BF01D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7D30AE3-80EC-004B-8D22-52B4C86CA52F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="340" yWindow="500" windowWidth="28100" windowHeight="16100" xr2:uid="{0BA294BD-C3A5-D442-BD2F-C06C5A9B2827}"/>
   </bookViews>
@@ -504,7 +504,7 @@
   <dimension ref="F2:M20"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>